<commit_message>
VRT Test Project Updated
</commit_message>
<xml_diff>
--- a/VRT/TestData/UserManagementTestData.xlsx
+++ b/VRT/TestData/UserManagementTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stored-Code\TestAutomation\Development\Root\Source\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7306E6F-8C3A-4027-89AF-8582F9DE8E72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F55239-74B3-4E80-A512-668C5E6D1360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="14" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
   <sheets>
     <sheet name="tcADMN124" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,13 @@
     <sheet name="tcADMN133" sheetId="6" r:id="rId6"/>
     <sheet name="tcADMN134" sheetId="7" r:id="rId7"/>
     <sheet name="tcADMN146" sheetId="8" r:id="rId8"/>
+    <sheet name="tcADMN146a" sheetId="9" r:id="rId9"/>
+    <sheet name="tcADMN147a" sheetId="12" r:id="rId10"/>
+    <sheet name="tcADMN150" sheetId="13" r:id="rId11"/>
+    <sheet name="tcADMN150a" sheetId="14" r:id="rId12"/>
+    <sheet name="tcADMN159" sheetId="17" r:id="rId13"/>
+    <sheet name="tcADMN160" sheetId="18" r:id="rId14"/>
+    <sheet name="tcADMN188a" sheetId="19" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -163,9 +170,6 @@
     <t>A3Q</t>
   </si>
   <si>
-    <t>User Id cannot be blank. Please provide a valid User Id</t>
-  </si>
-  <si>
     <t>Please select valid user type</t>
   </si>
   <si>
@@ -200,13 +204,151 @@
   </si>
   <si>
     <t>aaa</t>
+  </si>
+  <si>
+    <t>1##</t>
+  </si>
+  <si>
+    <t>$$</t>
+  </si>
+  <si>
+    <t>12T</t>
+  </si>
+  <si>
+    <t>12G</t>
+  </si>
+  <si>
+    <t>12J</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>12E</t>
+  </si>
+  <si>
+    <t>Title accepts only upper case , lower case and special character like hyphen, underscore and blank</t>
+  </si>
+  <si>
+    <t>Avv</t>
+  </si>
+  <si>
+    <t>att</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>fh</t>
+  </si>
+  <si>
+    <t>!@as</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Flag1</t>
+  </si>
+  <si>
+    <t>dfsd@fg.com</t>
+  </si>
+  <si>
+    <t>Flag2</t>
+  </si>
+  <si>
+    <t>Abbsggsgs</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>1$%</t>
+  </si>
+  <si>
+    <t>9*</t>
+  </si>
+  <si>
+    <t>!2</t>
+  </si>
+  <si>
+    <t>Flag9</t>
+  </si>
+  <si>
+    <t>Flag7</t>
+  </si>
+  <si>
+    <t>Phone accepts only numbers</t>
+  </si>
+  <si>
+    <t>9890983456</t>
+  </si>
+  <si>
+    <t>@domain.web</t>
+  </si>
+  <si>
+    <t>email@-10.17.17.100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Email..email@domain.com </t>
+  </si>
+  <si>
+    <t>Please enter a valid Email ID</t>
+  </si>
+  <si>
+    <t>ylag</t>
+  </si>
+  <si>
+    <t>ylag1</t>
+  </si>
+  <si>
+    <t>ylag2</t>
+  </si>
+  <si>
+    <t>ylag3</t>
+  </si>
+  <si>
+    <t>email@subdomain.domain.com</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test78@test.com</t>
+  </si>
+  <si>
+    <t>email@email.com</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>Test65</t>
+  </si>
+  <si>
+    <t>User Id cannot be blank. Please provide valid User Id.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +370,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +416,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -291,10 +453,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,8 +507,33 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,7 +849,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -756,7 +944,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,10 +964,807 @@
         <v>8</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB13E5F-2ECF-41C5-BE95-F394F239294C}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5335B6-CB8D-48D6-B8DE-668C59B57752}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>123</v>
+      </c>
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{AD9ADDC4-212E-46D9-82AB-293A110243D0}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{B1FE8B19-32AA-42C3-ABDE-812676E261ED}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{1503B510-2D2E-4E4B-AE07-D7A01F63ECAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300FA0F9-C58F-4C27-AA27-2C4C705A017F}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>123</v>
+      </c>
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>123</v>
+      </c>
+      <c r="D6" s="1">
+        <v>123</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{EA57F7E5-887A-4AEA-A8DA-CC820CE0A393}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{CC6112AE-8690-448A-8863-7B4BF48679F6}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{AA15A2E3-AAA0-41A8-A5F0-0A8C4A2AA377}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497D9F06-C61B-42E6-9F7B-8B3F90BB191B}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="23">
+        <v>576346674</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>123</v>
+      </c>
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{3EC98782-6F59-4D29-8DFF-1B8F7C52A76B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F292CD-DD2E-4F85-9B62-1ECD3B744AB0}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>123</v>
+      </c>
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{D02DE146-9FDA-4F62-9186-D852FA4DC1F3}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{A5A11028-AECF-46A4-BF80-AF57915538EF}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{D60A445B-9B49-46F7-A010-79D253AB1D41}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{376C4FF9-D6CE-49A7-944B-DD7C74735AA0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9AC851-843F-4311-966F-386BB924662B}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1091,7 +2076,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,25 +2459,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1504,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC3C7EE-407E-4327-AA5D-6BA458EBDC28}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,7 +2513,7 @@
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1537,7 +2522,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>32</v>
@@ -1549,7 +2534,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -1557,7 +2542,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>31</v>
@@ -1569,7 +2554,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -1589,7 +2574,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -1609,7 +2594,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
@@ -1618,4 +2603,166 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276B0B36-A61C-445F-BE6E-42C476FED9AF}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>324635</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{22916C02-9A54-4154-9B8E-55B78D691CE6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>